<commit_message>
an example project about manipulating excel
</commit_message>
<xml_diff>
--- a/python_excel/transactions.xlsx
+++ b/python_excel/transactions.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graymoka/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graymoka/github/pythontestproject/python_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8080FD4-4795-644A-91C1-BD1B2FABE214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CB4CDD-B07B-7F4C-A277-1554018200D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="11260" windowWidth="28040" windowHeight="16320" xr2:uid="{7C7DF51A-4D42-FA48-ACE4-3ADF65325FE0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" xr2:uid="{7C7DF51A-4D42-FA48-ACE4-3ADF65325FE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -398,7 +398,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -427,10 +427,7 @@
       <c r="C2" s="1">
         <v>5.95</v>
       </c>
-      <c r="E2" s="1">
-        <f>C2*0.9</f>
-        <v>5.3550000000000004</v>
-      </c>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
@@ -442,10 +439,7 @@
       <c r="C3" s="1">
         <v>6.95</v>
       </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E4" si="0">C3*0.9</f>
-        <v>6.2549999999999999</v>
-      </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
@@ -457,10 +451,7 @@
       <c r="C4" s="1">
         <v>7.95</v>
       </c>
-      <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>7.1550000000000002</v>
-      </c>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>